<commit_message>
Updated Test Data and Removed Flakiness
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhishekpuri/IdeaProjects/douglas/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D372C3-893B-1242-841B-2AE8BC792B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055E02D6-219C-6D4E-91B7-02DA9459DA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{A448E166-A043-E241-92AD-E81F96619FA6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19760" xr2:uid="{A448E166-A043-E241-92AD-E81F96619FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="ParfumProductFilterTest" sheetId="1" r:id="rId1"/>
@@ -129,10 +129,10 @@
     <t>Montblanc</t>
   </si>
   <si>
-    <t>Dior</t>
-  </si>
-  <si>
     <t>Eau de Parfum</t>
+  </si>
+  <si>
+    <t>DIOR</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +569,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -591,7 +591,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>

</xml_diff>